<commit_message>
importando dados da planilha
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>CPF</t>
   </si>
@@ -36,40 +36,40 @@
     <t>COMPROVANTE</t>
   </si>
   <si>
-    <t>00408731702</t>
-  </si>
-  <si>
-    <t>11061968</t>
-  </si>
-  <si>
-    <t>SEI-490002/001152/2025</t>
-  </si>
-  <si>
-    <t>RECEITA_IVONE</t>
-  </si>
-  <si>
-    <t>D:\PROJETOS EM ANDAMENTO\consulta_receita\PDFs\RECEITA_00408731702_RECEITA_IVONE.pdf</t>
-  </si>
-  <si>
-    <t>06957305767</t>
-  </si>
-  <si>
-    <t>27051976</t>
-  </si>
-  <si>
-    <t>sem sei</t>
-  </si>
-  <si>
-    <t>meu teste</t>
-  </si>
-  <si>
-    <t>D:\PROJETOS EM ANDAMENTO\consulta_receita\PDFs\RECEITA_06957305767_meu teste.pdf</t>
-  </si>
-  <si>
-    <t>SEGUNDA_VEZ</t>
-  </si>
-  <si>
-    <t>D:\PROJETOS EM ANDAMENTO\consulta_receita\PDFs\RECEITA_00408731702_SEGUNDA_VEZ.pdf</t>
+    <t>38895366700</t>
+  </si>
+  <si>
+    <t>10061953</t>
+  </si>
+  <si>
+    <t>SEI-490002/002287/2025</t>
+  </si>
+  <si>
+    <t>ANTÔNIO</t>
+  </si>
+  <si>
+    <t>D:\PROJETOS EM ANDAMENTO\consulta_receita\PDFs\RECEITA_38895366700_ANTÔNIO.pdf</t>
+  </si>
+  <si>
+    <t>79348289772</t>
+  </si>
+  <si>
+    <t>03041963</t>
+  </si>
+  <si>
+    <t>SEI-490002/001100/2025</t>
+  </si>
+  <si>
+    <t>ROSÂNGELA</t>
+  </si>
+  <si>
+    <t>D:\PROJETOS EM ANDAMENTO\consulta_receita\PDFs\RECEITA_79348289772_ROSÂNGELA.pdf</t>
+  </si>
+  <si>
+    <t>UNIDADE</t>
+  </si>
+  <si>
+    <t>SHF</t>
   </si>
 </sst>
 </file>
@@ -98,7 +98,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -121,13 +121,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -432,22 +446,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.140625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,8 +470,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -480,8 +490,11 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -497,21 +510,7 @@
       <c r="E3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>